<commit_message>
sprites en prefabs en planningen en zo
</commit_message>
<xml_diff>
--- a/Documents/Balancing.xlsx
+++ b/Documents/Balancing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yorick\Dungeon-Dweller\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431378B6-C46E-4980-B6CD-0F797D8DA961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3A696D-7115-4E83-A171-F3DC1C45D85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WeaponDMG" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="439">
   <si>
     <t>Fire:</t>
   </si>
@@ -781,15 +781,6 @@
     <t>Jasper Ring T3</t>
   </si>
   <si>
-    <t>Magic Damage + 1</t>
-  </si>
-  <si>
-    <t>Magic Damage + 2</t>
-  </si>
-  <si>
-    <t>Magic Damage + 3</t>
-  </si>
-  <si>
     <t>Ruby Ring T1</t>
   </si>
   <si>
@@ -799,15 +790,6 @@
     <t>Ruby Ring T3</t>
   </si>
   <si>
-    <t>Health Regeneration + 1</t>
-  </si>
-  <si>
-    <t>Health Regeneration + 2</t>
-  </si>
-  <si>
-    <t>Health Regeneration + 3</t>
-  </si>
-  <si>
     <t>Ring of Magma</t>
   </si>
   <si>
@@ -1346,6 +1328,39 @@
   </si>
   <si>
     <t>Blindness</t>
+  </si>
+  <si>
+    <t>Health + 3</t>
+  </si>
+  <si>
+    <t>Health  + 2</t>
+  </si>
+  <si>
+    <t>Strength + 3</t>
+  </si>
+  <si>
+    <t>Strength + 2</t>
+  </si>
+  <si>
+    <t>Onyx Ring T1</t>
+  </si>
+  <si>
+    <t>Onyx Ring T2</t>
+  </si>
+  <si>
+    <t>Onyx Ring T3</t>
+  </si>
+  <si>
+    <t>1 Onyx Gemstone</t>
+  </si>
+  <si>
+    <t>Defense + 3</t>
+  </si>
+  <si>
+    <t>Defense + 2</t>
+  </si>
+  <si>
+    <t>Defense + 1</t>
   </si>
 </sst>
 </file>
@@ -2085,7 +2100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2205,7 +2220,7 @@
         <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="E8" s="84" t="s">
         <v>210</v>
@@ -6087,7 +6102,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -6096,7 +6111,7 @@
         <v>500</v>
       </c>
       <c r="H13" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="I13">
         <f>C13/B13</f>
@@ -6113,7 +6128,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6136,7 +6151,7 @@
         <v>151</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -6150,7 +6165,7 @@
         <v>167</v>
       </c>
       <c r="G2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -6161,10 +6176,10 @@
         <v>163</v>
       </c>
       <c r="E3" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G3" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -6178,7 +6193,7 @@
         <v>168</v>
       </c>
       <c r="G4" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -6189,7 +6204,7 @@
         <v>166</v>
       </c>
       <c r="G5" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -6391,10 +6406,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F8B3FC-5D85-485F-A059-8EE46BCF745E}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6408,7 +6423,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B1">
         <v>22</v>
@@ -6425,10 +6440,10 @@
         <v>213</v>
       </c>
       <c r="D2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -6442,10 +6457,10 @@
         <v>215</v>
       </c>
       <c r="D3" s="85" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -6456,10 +6471,10 @@
         <v>221</v>
       </c>
       <c r="D4" s="86" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E4" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -6470,10 +6485,10 @@
         <v>219</v>
       </c>
       <c r="D5" s="86" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E5" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -6481,13 +6496,13 @@
         <v>220</v>
       </c>
       <c r="B6" t="s">
-        <v>239</v>
+        <v>438</v>
       </c>
       <c r="D6" s="86" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E6" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -6495,13 +6510,13 @@
         <v>222</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>437</v>
       </c>
       <c r="D7" s="87" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E7" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -6509,13 +6524,13 @@
         <v>223</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>436</v>
       </c>
       <c r="D8" s="85" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E8" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -6526,10 +6541,10 @@
         <v>227</v>
       </c>
       <c r="D9" s="86" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E9" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -6540,10 +6555,10 @@
         <v>228</v>
       </c>
       <c r="D10" s="87" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E10" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -6554,10 +6569,10 @@
         <v>229</v>
       </c>
       <c r="D11" s="85" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E11" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -6568,10 +6583,10 @@
         <v>233</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E12" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -6582,10 +6597,10 @@
         <v>234</v>
       </c>
       <c r="D13" s="87" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E13" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -6596,10 +6611,10 @@
         <v>235</v>
       </c>
       <c r="D14" s="85" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E14" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -6607,13 +6622,13 @@
         <v>236</v>
       </c>
       <c r="B15" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D15" s="86" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E15" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -6621,13 +6636,13 @@
         <v>237</v>
       </c>
       <c r="B16" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D16" s="87" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E16" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -6635,13 +6650,13 @@
         <v>238</v>
       </c>
       <c r="B17" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D17" s="85" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E17" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -6649,13 +6664,13 @@
         <v>242</v>
       </c>
       <c r="B18" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="D18" s="86" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E18" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -6663,13 +6678,13 @@
         <v>243</v>
       </c>
       <c r="B19" t="s">
-        <v>246</v>
+        <v>431</v>
       </c>
       <c r="D19" s="87" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E19" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -6677,576 +6692,618 @@
         <v>244</v>
       </c>
       <c r="B20" t="s">
-        <v>247</v>
+        <v>430</v>
       </c>
       <c r="D20" s="85" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E20" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>248</v>
+        <v>432</v>
       </c>
       <c r="B21" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="D21" s="86" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E21" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>249</v>
+        <v>433</v>
       </c>
       <c r="B22" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D22" s="87" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E22" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>250</v>
+        <v>434</v>
       </c>
       <c r="B23" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D23" s="85" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E23" t="s">
-        <v>273</v>
+        <v>435</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
       <c r="B24" t="s">
-        <v>286</v>
+        <v>219</v>
       </c>
       <c r="D24" s="86" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E24" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>284</v>
+        <v>246</v>
       </c>
       <c r="B25" t="s">
-        <v>287</v>
+        <v>429</v>
       </c>
       <c r="D25" s="87" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E25" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="B26" t="s">
-        <v>288</v>
+        <v>428</v>
       </c>
       <c r="D26" s="85" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E26" t="s">
-        <v>289</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="B27" t="s">
-        <v>255</v>
-      </c>
-      <c r="D27" s="87" t="s">
-        <v>259</v>
+        <v>280</v>
+      </c>
+      <c r="D27" s="86" t="s">
+        <v>250</v>
       </c>
       <c r="E27" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>364</v>
+        <v>278</v>
       </c>
       <c r="B28" t="s">
-        <v>309</v>
-      </c>
-      <c r="D28" s="86" t="s">
-        <v>256</v>
+        <v>281</v>
+      </c>
+      <c r="D28" s="87" t="s">
+        <v>253</v>
       </c>
       <c r="E28" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>365</v>
+        <v>279</v>
       </c>
       <c r="B29" t="s">
-        <v>310</v>
-      </c>
-      <c r="D29" s="87" t="s">
-        <v>259</v>
+        <v>282</v>
+      </c>
+      <c r="D29" s="85" t="s">
+        <v>252</v>
       </c>
       <c r="E29" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>366</v>
+        <v>248</v>
       </c>
       <c r="B30" t="s">
-        <v>327</v>
-      </c>
-      <c r="D30" s="85" t="s">
-        <v>258</v>
+        <v>249</v>
+      </c>
+      <c r="D30" s="87" t="s">
+        <v>253</v>
       </c>
       <c r="E30" t="s">
-        <v>338</v>
+        <v>254</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="B31" t="s">
-        <v>311</v>
-      </c>
-      <c r="D31" s="79" t="s">
-        <v>337</v>
+        <v>303</v>
+      </c>
+      <c r="D31" s="86" t="s">
+        <v>250</v>
       </c>
       <c r="E31" t="s">
-        <v>339</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>291</v>
+        <v>359</v>
       </c>
       <c r="B32" t="s">
-        <v>312</v>
-      </c>
-      <c r="D32" s="86" t="s">
-        <v>256</v>
+        <v>304</v>
+      </c>
+      <c r="D32" s="87" t="s">
+        <v>253</v>
       </c>
       <c r="E32" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>299</v>
+        <v>360</v>
       </c>
       <c r="B33" t="s">
-        <v>313</v>
-      </c>
-      <c r="D33" s="87" t="s">
-        <v>259</v>
+        <v>321</v>
+      </c>
+      <c r="D33" s="85" t="s">
+        <v>252</v>
       </c>
       <c r="E33" t="s">
-        <v>270</v>
+        <v>332</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>300</v>
+        <v>361</v>
       </c>
       <c r="B34" t="s">
-        <v>326</v>
-      </c>
-      <c r="D34" s="85" t="s">
-        <v>258</v>
+        <v>305</v>
+      </c>
+      <c r="D34" s="79" t="s">
+        <v>331</v>
       </c>
       <c r="E34" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>336</v>
+        <v>285</v>
       </c>
       <c r="B35" t="s">
-        <v>314</v>
-      </c>
-      <c r="D35" s="79" t="s">
-        <v>337</v>
+        <v>306</v>
+      </c>
+      <c r="D35" s="86" t="s">
+        <v>250</v>
       </c>
       <c r="E35" t="s">
-        <v>340</v>
+        <v>264</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B36" t="s">
-        <v>315</v>
-      </c>
-      <c r="D36" s="86" t="s">
-        <v>256</v>
+        <v>307</v>
+      </c>
+      <c r="D36" s="87" t="s">
+        <v>253</v>
       </c>
       <c r="E36" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="B37" t="s">
-        <v>316</v>
-      </c>
-      <c r="D37" s="87" t="s">
-        <v>259</v>
+        <v>320</v>
+      </c>
+      <c r="D37" s="85" t="s">
+        <v>252</v>
       </c>
       <c r="E37" t="s">
-        <v>270</v>
+        <v>338</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>302</v>
+        <v>330</v>
       </c>
       <c r="B38" t="s">
-        <v>325</v>
-      </c>
-      <c r="D38" s="85" t="s">
-        <v>258</v>
+        <v>308</v>
+      </c>
+      <c r="D38" s="79" t="s">
+        <v>331</v>
       </c>
       <c r="E38" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>335</v>
+        <v>284</v>
       </c>
       <c r="B39" t="s">
-        <v>320</v>
-      </c>
-      <c r="D39" s="79" t="s">
-        <v>337</v>
+        <v>309</v>
+      </c>
+      <c r="D39" s="86" t="s">
+        <v>250</v>
       </c>
       <c r="E39" t="s">
-        <v>341</v>
+        <v>264</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B40" t="s">
-        <v>321</v>
-      </c>
-      <c r="D40" s="86" t="s">
-        <v>256</v>
+        <v>310</v>
+      </c>
+      <c r="D40" s="87" t="s">
+        <v>253</v>
       </c>
       <c r="E40" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B41" t="s">
-        <v>317</v>
-      </c>
-      <c r="D41" s="87" t="s">
-        <v>259</v>
+        <v>319</v>
+      </c>
+      <c r="D41" s="85" t="s">
+        <v>252</v>
       </c>
       <c r="E41" t="s">
-        <v>270</v>
+        <v>339</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>304</v>
+        <v>329</v>
       </c>
       <c r="B42" t="s">
-        <v>324</v>
-      </c>
-      <c r="D42" s="85" t="s">
-        <v>258</v>
+        <v>314</v>
+      </c>
+      <c r="D42" s="79" t="s">
+        <v>331</v>
       </c>
       <c r="E42" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>334</v>
+        <v>286</v>
       </c>
       <c r="B43" t="s">
-        <v>322</v>
-      </c>
-      <c r="D43" s="79" t="s">
-        <v>337</v>
+        <v>315</v>
+      </c>
+      <c r="D43" s="86" t="s">
+        <v>250</v>
       </c>
       <c r="E43" t="s">
-        <v>342</v>
+        <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B44" t="s">
-        <v>323</v>
-      </c>
-      <c r="D44" s="86" t="s">
-        <v>256</v>
+        <v>311</v>
+      </c>
+      <c r="D44" s="87" t="s">
+        <v>253</v>
       </c>
       <c r="E44" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="B45" t="s">
         <v>318</v>
       </c>
-      <c r="D45" s="87" t="s">
-        <v>259</v>
+      <c r="D45" s="85" t="s">
+        <v>252</v>
       </c>
       <c r="E45" t="s">
-        <v>270</v>
+        <v>340</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>306</v>
+        <v>328</v>
       </c>
       <c r="B46" t="s">
-        <v>329</v>
-      </c>
-      <c r="D46" s="85" t="s">
-        <v>258</v>
+        <v>316</v>
+      </c>
+      <c r="D46" s="79" t="s">
+        <v>331</v>
       </c>
       <c r="E46" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>332</v>
+        <v>287</v>
       </c>
       <c r="B47" t="s">
-        <v>333</v>
-      </c>
-      <c r="D47" s="79" t="s">
-        <v>337</v>
+        <v>317</v>
+      </c>
+      <c r="D47" s="86" t="s">
+        <v>250</v>
       </c>
       <c r="E47" t="s">
-        <v>343</v>
+        <v>264</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B48" t="s">
-        <v>319</v>
-      </c>
-      <c r="D48" s="86" t="s">
-        <v>256</v>
+        <v>312</v>
+      </c>
+      <c r="D48" s="87" t="s">
+        <v>253</v>
       </c>
       <c r="E48" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="B49" t="s">
-        <v>319</v>
-      </c>
-      <c r="D49" s="87" t="s">
-        <v>259</v>
+        <v>323</v>
+      </c>
+      <c r="D49" s="85" t="s">
+        <v>252</v>
       </c>
       <c r="E49" t="s">
-        <v>270</v>
+        <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>308</v>
+        <v>326</v>
       </c>
       <c r="B50" t="s">
-        <v>328</v>
-      </c>
-      <c r="D50" s="85" t="s">
-        <v>258</v>
+        <v>327</v>
+      </c>
+      <c r="D50" s="79" t="s">
+        <v>331</v>
       </c>
       <c r="E50" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>330</v>
+        <v>288</v>
       </c>
       <c r="B51" t="s">
-        <v>331</v>
-      </c>
-      <c r="D51" s="79" t="s">
-        <v>337</v>
+        <v>313</v>
+      </c>
+      <c r="D51" s="86" t="s">
+        <v>250</v>
       </c>
       <c r="E51" t="s">
-        <v>349</v>
+        <v>264</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>369</v>
+        <v>301</v>
       </c>
       <c r="B52" t="s">
-        <v>370</v>
-      </c>
-      <c r="D52" s="85" t="s">
-        <v>258</v>
+        <v>313</v>
+      </c>
+      <c r="D52" s="87" t="s">
+        <v>253</v>
       </c>
       <c r="E52" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>395</v>
+        <v>302</v>
       </c>
       <c r="B53" t="s">
-        <v>415</v>
+        <v>322</v>
       </c>
       <c r="D53" s="85" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E53" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>429</v>
-      </c>
-      <c r="B65" t="s">
-        <v>431</v>
-      </c>
-      <c r="D65" s="34" t="s">
-        <v>297</v>
-      </c>
-      <c r="E65" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>324</v>
+      </c>
+      <c r="B54" t="s">
+        <v>325</v>
+      </c>
+      <c r="D54" s="79" t="s">
+        <v>331</v>
+      </c>
+      <c r="E54" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>363</v>
       </c>
-      <c r="B66" t="s">
-        <v>359</v>
-      </c>
-      <c r="D66" s="34" t="s">
-        <v>297</v>
-      </c>
-      <c r="E66" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>354</v>
-      </c>
-      <c r="B67" t="s">
-        <v>270</v>
-      </c>
-      <c r="D67" s="34" t="s">
-        <v>297</v>
-      </c>
-      <c r="E67" t="s">
-        <v>353</v>
+      <c r="B55" t="s">
+        <v>364</v>
+      </c>
+      <c r="D55" s="85" t="s">
+        <v>252</v>
+      </c>
+      <c r="E55" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>389</v>
+      </c>
+      <c r="B56" t="s">
+        <v>409</v>
+      </c>
+      <c r="D56" s="85" t="s">
+        <v>252</v>
+      </c>
+      <c r="E56" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>295</v>
+        <v>423</v>
       </c>
       <c r="B68" t="s">
-        <v>296</v>
+        <v>425</v>
       </c>
       <c r="D68" s="34" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E68" t="s">
-        <v>348</v>
+        <v>426</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B69" t="s">
-        <v>350</v>
-      </c>
-      <c r="D69" s="88" t="s">
-        <v>351</v>
+        <v>353</v>
+      </c>
+      <c r="D69" s="34" t="s">
+        <v>291</v>
       </c>
       <c r="E69" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>348</v>
+      </c>
+      <c r="B70" t="s">
         <v>264</v>
       </c>
-      <c r="B70" t="s">
-        <v>360</v>
-      </c>
-      <c r="D70" s="81" t="s">
-        <v>265</v>
+      <c r="D70" s="34" t="s">
+        <v>291</v>
       </c>
       <c r="E70" t="s">
-        <v>270</v>
+        <v>347</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="B71" t="s">
-        <v>262</v>
-      </c>
-      <c r="C71" t="s">
-        <v>298</v>
-      </c>
-      <c r="D71" s="77" t="s">
-        <v>263</v>
+        <v>290</v>
+      </c>
+      <c r="D71" s="34" t="s">
+        <v>291</v>
       </c>
       <c r="E71" t="s">
-        <v>270</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>355</v>
+      </c>
+      <c r="B72" t="s">
+        <v>344</v>
+      </c>
+      <c r="D72" s="88" t="s">
+        <v>345</v>
+      </c>
+      <c r="E72" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>258</v>
+      </c>
+      <c r="B73" t="s">
+        <v>354</v>
+      </c>
+      <c r="D73" s="81" t="s">
+        <v>259</v>
+      </c>
+      <c r="E73" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>255</v>
+      </c>
+      <c r="B74" t="s">
+        <v>256</v>
+      </c>
+      <c r="C74" t="s">
+        <v>292</v>
+      </c>
+      <c r="D74" s="77" t="s">
+        <v>257</v>
+      </c>
+      <c r="E74" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -7281,61 +7338,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="86" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="B1" s="90" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="C1" s="91" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="E1" s="90" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="F1" s="91" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="H1" s="90" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="I1" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="J1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="K1" s="90" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="L1" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="M1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="N1" s="90" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="O1" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="P1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="Q1" s="90" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="R1" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="S1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -7353,31 +7410,31 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="86" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B3" s="90" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C3" s="92" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D3" s="25">
         <v>2</v>
       </c>
       <c r="E3" s="90" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="F3" s="92" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="G3" s="25">
         <v>1</v>
       </c>
       <c r="H3" s="90" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="I3" s="89" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -7388,31 +7445,31 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="86" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="B4" s="90" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C4" s="91" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D4" s="25">
         <v>4</v>
       </c>
       <c r="E4" s="90" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="F4" s="91" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="G4" s="25">
         <v>1</v>
       </c>
       <c r="H4" s="90" t="s">
+        <v>372</v>
+      </c>
+      <c r="I4" t="s">
         <v>378</v>
-      </c>
-      <c r="I4" t="s">
-        <v>384</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -7423,31 +7480,31 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="86" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B5" s="90" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C5" s="91" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D5" s="25">
         <v>2</v>
       </c>
       <c r="E5" s="90" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="F5" s="91" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="G5" s="25">
         <v>2</v>
       </c>
       <c r="H5" s="90" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="I5" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -7458,22 +7515,22 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="86" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="B6" s="90" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C6" s="91" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D6" s="25">
         <v>2</v>
       </c>
       <c r="E6" s="90" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="F6" s="91" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="G6" s="25">
         <v>1</v>
@@ -7485,31 +7542,31 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="86" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="B7" s="90" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C7" s="91" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="D7" s="25">
         <v>3</v>
       </c>
       <c r="E7" s="90" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="F7" s="91" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="G7" s="25">
         <v>1</v>
       </c>
       <c r="H7" s="90" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="I7" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -7520,22 +7577,22 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="86" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="B8" s="90" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C8" s="91" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="D8" s="25">
         <v>3</v>
       </c>
       <c r="E8" s="90" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="F8" s="91" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="G8" s="25">
         <v>1</v>
@@ -7547,22 +7604,22 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="86" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="B9" s="90" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C9" s="91" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="D9" s="25">
         <v>5</v>
       </c>
       <c r="E9" s="90" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="F9" s="91" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="G9" s="25">
         <v>1</v>
@@ -7574,31 +7631,31 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="86" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="B10" s="90" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C10" s="91" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D10" s="25">
         <v>1</v>
       </c>
       <c r="E10" s="90" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="F10" s="91" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="G10" s="25">
         <v>1</v>
       </c>
       <c r="H10" s="90" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="I10" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -7609,58 +7666,58 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="86" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="B11" s="90" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C11" s="91" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="D11" s="25">
         <v>1</v>
       </c>
       <c r="E11" s="90" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="F11" s="91" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="G11" s="25">
         <v>2</v>
       </c>
       <c r="H11" s="90" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="I11" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11" s="90" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="L11" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="M11">
         <v>1</v>
       </c>
       <c r="N11" s="90" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="O11" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="P11">
         <v>1</v>
       </c>
       <c r="Q11" s="90" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="R11" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="S11">
         <v>1</v>
@@ -7668,29 +7725,29 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="86" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="C12" s="91" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D12" s="25">
         <v>1</v>
       </c>
       <c r="E12" s="90" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="F12" s="91" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="90" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="I12" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -7701,58 +7758,58 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="86" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="B13" s="90" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="C13" s="91" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="D13" s="25">
         <v>3</v>
       </c>
       <c r="E13" s="90" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="F13" s="91" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="G13" s="25">
         <v>1</v>
       </c>
       <c r="H13" s="90" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="I13" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="J13">
         <v>3</v>
       </c>
       <c r="K13" s="90" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="L13" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13" s="90" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="O13" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="P13">
         <v>1</v>
       </c>
       <c r="Q13" s="90" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="R13" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="S13">
         <v>1</v>
@@ -7760,61 +7817,61 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="86" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="B14" s="90" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C14" s="91" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="D14" s="25">
         <v>3</v>
       </c>
       <c r="E14" s="90" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="F14" s="91" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="G14" s="25">
         <v>1</v>
       </c>
       <c r="H14" s="90" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="I14" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="J14">
         <v>4</v>
       </c>
       <c r="K14" s="90" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="L14" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="M14">
         <v>1</v>
       </c>
       <c r="N14" s="90" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="O14" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="Q14" s="90"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="86" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="B15" s="90" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C15" s="91" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="D15" s="25">
         <v>1</v>
@@ -7868,7 +7925,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="86" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B19" s="90"/>
       <c r="C19" s="91"/>
@@ -7909,7 +7966,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="86" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B22" s="90"/>
       <c r="C22" s="91"/>
@@ -7950,7 +8007,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="86" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B25" s="90"/>
       <c r="C25" s="91"/>
@@ -7978,7 +8035,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="86" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B27" s="90"/>
       <c r="C27" s="91"/>
@@ -8012,26 +8069,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="B1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="B3" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>